<commit_message>
Commit Home Sunday_28-Jul-2024 16:17
</commit_message>
<xml_diff>
--- a/ClassestobeUsed.xlsx
+++ b/ClassestobeUsed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W10User\Documents\OnlineRepositories\InstallMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26DE028-B41B-434A-988D-95CB8189BCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E32F999-5C1C-4FD2-BED9-35986EE324E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="3270" windowWidth="21600" windowHeight="11370" xr2:uid="{1ED3A49F-F648-4EB7-9D0B-212075C0F798}"/>
+    <workbookView xWindow="4245" yWindow="1575" windowWidth="21600" windowHeight="11370" xr2:uid="{1ED3A49F-F648-4EB7-9D0B-212075C0F798}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -178,6 +178,48 @@
   </si>
   <si>
     <t>Win32_PhysicalMemory</t>
+  </si>
+  <si>
+    <t>NIC</t>
+  </si>
+  <si>
+    <t>CIM_NetworkAdapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AdapterType </t>
+  </si>
+  <si>
+    <t>Ethernet 802.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AdapterTypeId </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
+  </si>
+  <si>
+    <t>Realtek PCIe GbE Family Controller</t>
+  </si>
+  <si>
+    <t>MACAddress</t>
+  </si>
+  <si>
+    <t>30:24:A9:7D:D4:F8</t>
+  </si>
+  <si>
+    <t>Realtek</t>
+  </si>
+  <si>
+    <t>NetConnectionID</t>
+  </si>
+  <si>
+    <t>Ethernet</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>PhysicalAdapter</t>
   </si>
 </sst>
 </file>
@@ -207,12 +249,24 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -307,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -358,17 +412,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFAFBCB-B9E4-48BC-B4EB-1E5144B60BDB}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,20 +768,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="4"/>
@@ -907,6 +976,12 @@
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="E21" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -915,6 +990,12 @@
       <c r="B22" s="13" t="s">
         <v>33</v>
       </c>
+      <c r="E22" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
@@ -923,6 +1004,12 @@
       <c r="B23" s="13" t="s">
         <v>35</v>
       </c>
+      <c r="E23" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
@@ -931,6 +1018,12 @@
       <c r="B24" s="13" t="s">
         <v>37</v>
       </c>
+      <c r="E24" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
@@ -939,6 +1032,12 @@
       <c r="B25" s="13" t="s">
         <v>41</v>
       </c>
+      <c r="E25" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -947,6 +1046,12 @@
       <c r="B26" s="13" t="s">
         <v>38</v>
       </c>
+      <c r="E26" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
@@ -955,12 +1060,24 @@
       <c r="B27" s="13" t="s">
         <v>39</v>
       </c>
+      <c r="E27" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="13"/>
+      <c r="E28" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
@@ -969,6 +1086,12 @@
       <c r="B29" s="13">
         <v>2667</v>
       </c>
+      <c r="E29" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -977,6 +1100,12 @@
       <c r="B30" s="13">
         <v>26</v>
       </c>
+      <c r="E30" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="28" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
@@ -985,6 +1114,28 @@
       <c r="B31" s="15">
         <v>12</v>
       </c>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Commit Home Sunday_28-Jul-2024 22:13
</commit_message>
<xml_diff>
--- a/ClassestobeUsed.xlsx
+++ b/ClassestobeUsed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W10User\Documents\OnlineRepositories\InstallMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E32F999-5C1C-4FD2-BED9-35986EE324E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1BDB7C-F5EF-4A1B-B8DC-A84516210320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="1575" windowWidth="21600" windowHeight="11370" xr2:uid="{1ED3A49F-F648-4EB7-9D0B-212075C0F798}"/>
+    <workbookView xWindow="5700" yWindow="2325" windowWidth="21600" windowHeight="12975" xr2:uid="{1ED3A49F-F648-4EB7-9D0B-212075C0F798}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -220,12 +220,51 @@
   </si>
   <si>
     <t>PhysicalAdapter</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>21503C443413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SerialNumber </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MediaType </t>
+  </si>
+  <si>
+    <t>Fixed hard disk media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeviceID </t>
+  </si>
+  <si>
+    <t>\\.\PHYSICALDRIVE1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InterfaceType </t>
+  </si>
+  <si>
+    <t>SCSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Standard disk drives)</t>
+  </si>
+  <si>
+    <t>WDC  WDS100T2B0A-00SM50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,13 +282,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FFA31515"/>
       <name val="CaskaydiaCove Nerd Font Mono"/>
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +305,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,14 +407,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -376,18 +416,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,45 +431,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,389 +792,448 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFAFBCB-B9E4-48BC-B4EB-1E5144B60BDB}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="9" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="9" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="9" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="9" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="11" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="E10" s="7" t="s">
+      <c r="B10" s="8"/>
+      <c r="E10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="13"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="E12" s="7" t="s">
+      <c r="B12" s="8"/>
+      <c r="E12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="13"/>
-      <c r="E13" s="7" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="8"/>
+      <c r="E13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15" s="7" t="s">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E16" s="7" t="s">
+      <c r="A16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="7" t="s">
+      <c r="A17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="14" t="s">
+      <c r="A18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="E23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="8">
+        <v>2667</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="8">
+        <v>26</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="10">
+        <v>12</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="25" t="s">
+      <c r="E29" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26" s="26" t="s">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="23">
+        <v>1000202273280</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="B34" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="E28" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="13">
-        <v>2667</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="13">
-        <v>26</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="15">
-        <v>12</v>
-      </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
+      <c r="B35" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Commit Office Monday_29-Jul-2024 14:24
</commit_message>
<xml_diff>
--- a/ClassestobeUsed.xlsx
+++ b/ClassestobeUsed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W10User\Documents\OnlineRepositories\InstallMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1BDB7C-F5EF-4A1B-B8DC-A84516210320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942B4164-E0ED-4F6F-820B-6FFBC874BC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="2325" windowWidth="21600" windowHeight="12975" xr2:uid="{1ED3A49F-F648-4EB7-9D0B-212075C0F798}"/>
+    <workbookView xWindow="-17205" yWindow="930" windowWidth="14970" windowHeight="11505" xr2:uid="{1ED3A49F-F648-4EB7-9D0B-212075C0F798}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +434,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -443,41 +478,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -794,11 +794,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFAFBCB-B9E4-48BC-B4EB-1E5144B60BDB}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
@@ -806,33 +806,33 @@
     <col min="6" max="6" width="40.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A1" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -841,14 +841,14 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -857,65 +857,65 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="17" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="17" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1"/>
-      <c r="B6" s="26"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="27"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="21" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="9" spans="1:6">
+      <c r="A9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -925,7 +925,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
@@ -939,7 +939,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -951,7 +951,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="5"/>
       <c r="B13" s="8"/>
       <c r="E13" s="5" t="s">
@@ -961,7 +961,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>4</v>
       </c>
@@ -975,7 +975,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
       <c r="E15" s="5" t="s">
         <v>0</v>
       </c>
@@ -983,11 +983,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -997,7 +997,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
         <v>4</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1">
       <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1">
       <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
@@ -1041,21 +1041,21 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="5" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="5" t="s">
         <v>43</v>
       </c>
@@ -1095,80 +1095,80 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="8">
         <v>26</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="16" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1">
       <c r="A26" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="10">
         <v>12</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="17" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="20" t="s">
+    <row r="27" spans="1:6">
+      <c r="E27" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="19" t="s">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1">
+      <c r="E28" s="16" t="s">
         <v>58</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+    <row r="29" spans="1:6">
+      <c r="A29" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A30" s="17" t="s">
         <v>64</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="F30" s="22" t="b">
+      <c r="F30" s="19" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+    <row r="31" spans="1:6">
+      <c r="A31" s="17" t="s">
         <v>65</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -1177,18 +1177,18 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+    <row r="32" spans="1:6">
+      <c r="A32" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B32" s="20">
         <v>1000202273280</v>
       </c>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="17" t="s">
         <v>68</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -1197,8 +1197,8 @@
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+    <row r="34" spans="1:6">
+      <c r="A34" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -1207,8 +1207,8 @@
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
+    <row r="35" spans="1:6">
+      <c r="A35" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -1217,8 +1217,8 @@
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="24" t="s">
+    <row r="36" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A36" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -1227,11 +1227,11 @@
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
     </row>

</xml_diff>